<commit_message>
Update deployment expedia & multiple producttype dispatcher
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Expedia/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Expedia/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Expedia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C458CC-10F7-479F-9F24-61369C3FBA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A500ACEF-AB6D-407E-92AB-D3E93E8AB84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="3552" windowWidth="21588" windowHeight="10620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23232" windowHeight="11496" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -185,7 +185,10 @@
     <t>PathSAKey</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_UploadBucket</t>
+    <t>Captcha_SiteKey</t>
+  </si>
+  <si>
+    <t>Captcha_RuleId</t>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
@@ -197,37 +200,52 @@
     <t>DialogDownloadChrome</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathDownloadChrome</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_DialogDownloadChrome</t>
-  </si>
-  <si>
     <t>SenderName</t>
   </si>
   <si>
     <t>RPA_Moon_SenderName</t>
   </si>
   <si>
+    <t>RPA_Moon_Captcha_RuleId</t>
+  </si>
+  <si>
+    <t>RPA_Moon_GCaptcha_RuleId</t>
+  </si>
+  <si>
+    <t>GCaptcha_RuleId</t>
+  </si>
+  <si>
+    <t>RPA021_MOLPAY_Captcha_SiteKey</t>
+  </si>
+  <si>
+    <t>RPA_Moon_Cred_Gmail</t>
+  </si>
+  <si>
+    <t>RPA_Moon_UploadBucket</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathDownloadChrome</t>
+  </si>
+  <si>
+    <t>RPA_Moon_DialogDownloadChrome</t>
+  </si>
+  <si>
+    <t>FlagError</t>
+  </si>
+  <si>
     <t>RPA090_Expedia_FlagError</t>
   </si>
   <si>
-    <t>FlagError</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_Cred_Gmail</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_SheetIdConfig_Accommodation</t>
+    <t>RPA_Moon_SheetIdConfig_Accommodation</t>
   </si>
 </sst>
 </file>
@@ -604,11 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -655,10 +672,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.3" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -695,8 +712,8 @@
       <c r="A7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>63</v>
+      <c r="B7" t="s">
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
@@ -704,10 +721,10 @@
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1"/>
@@ -1702,9 +1719,6 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -2873,7 +2887,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -2928,7 +2942,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
@@ -2936,7 +2950,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -2944,7 +2958,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -2952,23 +2966,23 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
@@ -2976,12 +2990,33 @@
         <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.3" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.3" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.3" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.3" customHeight="1"/>
@@ -3968,8 +4003,14 @@
     <row r="995" ht="14.3" customHeight="1"/>
     <row r="996" ht="14.3" customHeight="1"/>
     <row r="997" ht="14.3" customHeight="1"/>
+    <row r="998" ht="14.3" customHeight="1"/>
+    <row r="999" ht="14.3" customHeight="1"/>
+    <row r="1000" ht="14.3" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update upload file to gdrive
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Expedia/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Expedia/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Expedia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A500ACEF-AB6D-407E-92AB-D3E93E8AB84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C458CC-10F7-479F-9F24-61369C3FBA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23232" windowHeight="11496" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3552" yWindow="3552" windowWidth="21588" windowHeight="10620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -185,10 +185,7 @@
     <t>PathSAKey</t>
   </si>
   <si>
-    <t>Captcha_SiteKey</t>
-  </si>
-  <si>
-    <t>Captcha_RuleId</t>
+    <t>[Dev] RPA_Moon_UploadBucket</t>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
@@ -200,52 +197,37 @@
     <t>DialogDownloadChrome</t>
   </si>
   <si>
+    <t>[Dev] RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathDownloadChrome</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_DialogDownloadChrome</t>
+  </si>
+  <si>
     <t>SenderName</t>
   </si>
   <si>
     <t>RPA_Moon_SenderName</t>
   </si>
   <si>
-    <t>RPA_Moon_Captcha_RuleId</t>
-  </si>
-  <si>
-    <t>RPA_Moon_GCaptcha_RuleId</t>
-  </si>
-  <si>
-    <t>GCaptcha_RuleId</t>
-  </si>
-  <si>
-    <t>RPA021_MOLPAY_Captcha_SiteKey</t>
-  </si>
-  <si>
-    <t>RPA_Moon_Cred_Gmail</t>
-  </si>
-  <si>
-    <t>RPA_Moon_UploadBucket</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathDownloadChrome</t>
-  </si>
-  <si>
-    <t>RPA_Moon_DialogDownloadChrome</t>
+    <t>RPA090_Expedia_FlagError</t>
   </si>
   <si>
     <t>FlagError</t>
   </si>
   <si>
-    <t>RPA090_Expedia_FlagError</t>
-  </si>
-  <si>
-    <t>RPA_Moon_SheetIdConfig_Accommodation</t>
+    <t>[Dev] RPA_Moon_Cred_Gmail</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_Accommodation</t>
   </si>
 </sst>
 </file>
@@ -622,10 +604,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -672,10 +655,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.3" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -712,8 +695,8 @@
       <c r="A7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" t="s">
-        <v>61</v>
+      <c r="B7" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
@@ -721,10 +704,10 @@
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1"/>
@@ -1719,6 +1702,9 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <customProperties>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -2887,7 +2873,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -2942,7 +2928,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
@@ -2950,7 +2936,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -2958,7 +2944,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -2966,23 +2952,23 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
@@ -2990,33 +2976,12 @@
         <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.3" customHeight="1">
-      <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.3" customHeight="1">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.3" customHeight="1">
-      <c r="A11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-    </row>
+    <row r="9" spans="1:26" ht="14.3" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.3" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.3" customHeight="1"/>
@@ -4003,14 +3968,8 @@
     <row r="995" ht="14.3" customHeight="1"/>
     <row r="996" ht="14.3" customHeight="1"/>
     <row r="997" ht="14.3" customHeight="1"/>
-    <row r="998" ht="14.3" customHeight="1"/>
-    <row r="999" ht="14.3" customHeight="1"/>
-    <row r="1000" ht="14.3" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>